<commit_message>
Update the risk list
</commit_message>
<xml_diff>
--- a/docs/Project Management/Risk List.xlsx
+++ b/docs/Project Management/Risk List.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="119">
   <si>
     <t>Version</t>
   </si>
@@ -347,6 +347,9 @@
   </si>
   <si>
     <t>Issues with third-party components, such as libraries or frameworks, causing delays or failures.</t>
+  </si>
+  <si>
+    <t>Keep third-party components up to date. Regularly check for new versions and patches.</t>
   </si>
   <si>
     <t>R19</t>
@@ -2861,7 +2864,7 @@
         <v>63</v>
       </c>
       <c r="J20" s="24" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="K20" s="25"/>
       <c r="L20" s="25"/>
@@ -2882,19 +2885,19 @@
     </row>
     <row r="21">
       <c r="A21" s="16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B21" s="17">
         <v>45018.0</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F21" s="20">
         <v>5.0</v>
@@ -2910,7 +2913,7 @@
         <v>63</v>
       </c>
       <c r="J21" s="19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="K21" s="25"/>
       <c r="L21" s="25"/>
@@ -2931,19 +2934,19 @@
     </row>
     <row r="22">
       <c r="A22" s="16" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B22" s="17">
         <v>45018.0</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F22" s="20">
         <v>3.0</v>
@@ -2959,7 +2962,7 @@
         <v>63</v>
       </c>
       <c r="J22" s="19" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K22" s="25"/>
       <c r="L22" s="25"/>

</xml_diff>

<commit_message>
Update the missing item in the risk list
</commit_message>
<xml_diff>
--- a/docs/Project Management/Risk List.xlsx
+++ b/docs/Project Management/Risk List.xlsx
@@ -2464,10 +2464,12 @@
       <c r="F12" s="20">
         <v>5.0</v>
       </c>
-      <c r="G12" s="27"/>
+      <c r="G12" s="21">
+        <v>0.15</v>
+      </c>
       <c r="H12" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="I12" s="23" t="s">
         <v>34</v>

</xml_diff>